<commit_message>
Diego Saavedra - Se corrige generacion de Plantilla Futbol 8
</commit_message>
<xml_diff>
--- a/JCA_Futbol_Admin/Utiles/PlanillaFutbol8.xlsx
+++ b/JCA_Futbol_Admin/Utiles/PlanillaFutbol8.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\vive-tu-futbol\JCA_Futbol_Admin\Utiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7340" tabRatio="664"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
-    <sheet name="PLANILLA FUTBOL8" sheetId="6" r:id="rId1"/>
+    <sheet name="PLANILLA FUTBOL8" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'PLANILLA FUTBOL8'!$C$1:$P$51</definedName>
@@ -22,15 +22,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
-    <t>CAMPO</t>
+    <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t>HORA</t>
+    <t>COPA futbol 8 Y  11 2017</t>
   </si>
   <si>
-    <t>R</t>
+    <t xml:space="preserve">             vive tu fútbol planilla de juego</t>
+  </si>
+  <si>
+    <t>escenario</t>
   </si>
   <si>
     <t xml:space="preserve">    FECHA</t>
@@ -39,10 +42,46 @@
     <t>CATEGORÍA</t>
   </si>
   <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>UNICA</t>
+  </si>
+  <si>
+    <t>CAMPO</t>
+  </si>
+  <si>
+    <t>COPA</t>
+  </si>
+  <si>
+    <t>HORA</t>
+  </si>
+  <si>
+    <t>GRUPO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EQUIPO </t>
+  </si>
+  <si>
+    <t>Equipo1 de prua pruebas para siempre</t>
+  </si>
+  <si>
+    <t>equipo2</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
     <t>EQUIPO LOCAL</t>
   </si>
   <si>
-    <t>EQUIPO VISITANTE</t>
+    <t>CARNET</t>
   </si>
   <si>
     <t>GOL</t>
@@ -51,10 +90,25 @@
     <t>A</t>
   </si>
   <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>EQUIPO VISITANTE</t>
+  </si>
+  <si>
+    <t>carnet</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t>FIRMA CAPITÁN</t>
   </si>
   <si>
     <t xml:space="preserve">  FIRMA TÉCNICO</t>
+  </si>
+  <si>
+    <t>balon</t>
   </si>
   <si>
     <t>TOTALES GOLES :</t>
@@ -71,163 +125,97 @@
   <si>
     <t xml:space="preserve">        ASISTENTE Nº 2</t>
   </si>
-  <si>
-    <t xml:space="preserve">             vive tu fútbol planilla de juego</t>
-  </si>
-  <si>
-    <t>balon</t>
-  </si>
-  <si>
-    <t>escenario</t>
-  </si>
-  <si>
-    <t>CARNET</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>carnet</t>
-  </si>
-  <si>
-    <t>UNICA</t>
-  </si>
-  <si>
-    <t>COPA</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
-    <t>GRUPO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EQUIPO </t>
-  </si>
-  <si>
-    <t>COPA futbol 8 Y  11 2017</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
-  </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <i/>
       <sz val="22"/>
+      <color rgb="FF000000"/>
       <name val="Castellar"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color indexed="16"/>
+      <color rgb="FF800000"/>
       <name val="Arial"/>
-      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Castellar"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Castellar"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <color rgb="FF000000"/>
+      <name val="Castellar"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Castellar"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Century Gothic"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Castellar"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="30"/>
+      <color rgb="FF000000"/>
+      <name val="Castellar"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Castellar"/>
     </font>
     <font>
       <b/>
       <sz val="22"/>
+      <color rgb="FF000000"/>
       <name val="Castellar"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="24"/>
-      <name val="Castellar"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Castellar"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Castellar"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="26"/>
-      <name val="Castellar"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="24"/>
-      <name val="Castellar"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="30"/>
-      <name val="Castellar"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <name val="Castellar"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
   </fills>
-  <borders count="64">
+  <borders count="60">
     <border>
       <left/>
       <right/>
@@ -236,93 +224,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </left>
       <right/>
       <top style="double">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -331,7 +238,7 @@
       <left/>
       <right/>
       <top style="double">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -339,17 +246,17 @@
     <border>
       <left/>
       <right style="double">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="double">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="double">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </left>
       <right/>
       <top/>
@@ -359,160 +266,215 @@
     <border>
       <left/>
       <right style="double">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color indexed="8"/>
-      </left>
+      <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="double">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="8"/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
       </top>
-      <bottom style="thick">
-        <color indexed="8"/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="double">
-        <color indexed="8"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="double">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="double">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </left>
-      <right/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thick">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="double">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="double">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -520,23 +482,23 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -545,64 +507,64 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="double">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="double">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="double">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </left>
       <right/>
       <top/>
       <bottom style="double">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -611,31 +573,44 @@
       <right/>
       <top/>
       <bottom style="double">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="double">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </right>
       <top/>
       <bottom style="double">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thick">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -643,56 +618,69 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thick">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thick">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="double">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thick">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="double">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="double">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top/>
       <bottom/>
@@ -700,46 +688,46 @@
     </border>
     <border>
       <left style="double">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thick">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thick">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="double">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thick">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -747,49 +735,49 @@
       <left/>
       <right/>
       <top style="thick">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thick">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right/>
       <top style="thick">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="double">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thick">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -797,466 +785,392 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thick">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="double">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thick">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right/>
       <top style="thick">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thick">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thick">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thick">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="double">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="double">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thick">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thick">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="double">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right/>
       <top style="thick">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thick">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right/>
-      <top style="thick">
-        <color indexed="8"/>
+      <top style="thin">
+        <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
-      <top style="thick">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="double">
-        <color indexed="8"/>
-      </right>
-      <top style="thick">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thick">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="108">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="18" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="18" fontId="10" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="18" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="18" fontId="10" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="57" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="58" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="60" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="62" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="63" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Millares 2" xfId="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 2 2" xfId="3"/>
-    <cellStyle name="Normal 3" xfId="4"/>
-    <cellStyle name="Normal 3 2" xfId="5"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1270,291 +1184,77 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>31750</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>412750</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="86241" name="Line 1"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeShapeType="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm flipV="1">
-          <a:off x="4095750" y="16840200"/>
-          <a:ext cx="2101850" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:noFill/>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>698500</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="86242" name="Line 2"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeShapeType="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="450850" y="16840200"/>
-          <a:ext cx="1581150" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:noFill/>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>266700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>266700</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="86243" name="Line 3"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeShapeType="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm flipV="1">
-          <a:off x="7213600" y="16833850"/>
-          <a:ext cx="3619500" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:noFill/>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>107950</xdr:colOff>
+      <xdr:colOff>104775</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>736600</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>196850</xdr:rowOff>
-    </xdr:to>
+    <xdr:ext cx="962025" cy="828675"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="86244" name="7 Imagen"/>
+        <xdr:cNvPr id="2" name="7 Imagen"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="209550" y="95250"/>
-          <a:ext cx="965200" cy="825500"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>596900</xdr:colOff>
+      <xdr:colOff>600075</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>273050</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>209550</xdr:rowOff>
-    </xdr:to>
+    <xdr:ext cx="1000125" cy="866775"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="86245" name="8 Imagen"/>
+        <xdr:cNvPr id="3" name="8 Imagen"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="9753600" y="69850"/>
-          <a:ext cx="1003300" cy="863600"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1628,6 +1328,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1662,6 +1363,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1831,70 +1533,7 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1" cy="1"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst/>
-        </a:custGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-        <a:effectLst/>
-      </a:spPr>
-      <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
-      <a:lstStyle/>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1" cy="1"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst/>
-        </a:custGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-        <a:effectLst/>
-      </a:spPr>
-      <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
-      <a:lstStyle/>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
@@ -1903,14 +1542,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U269"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" topLeftCell="C22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="0.1796875" customWidth="1"/>
-    <col min="2" max="2" width="1.26953125" customWidth="1"/>
+    <col min="1" max="1" width="16" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="33.7265625" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="4.81640625" customWidth="1"/>
     <col min="4" max="4" width="12.81640625" customWidth="1"/>
     <col min="5" max="5" width="28.54296875" customWidth="1"/>
@@ -1927,9 +1566,9 @@
     <col min="16" max="16" width="5.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:17" ht="5.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:17" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="3" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -1965,7 +1604,7 @@
       <c r="C3" s="6"/>
       <c r="D3" s="8"/>
       <c r="E3" s="67" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="F3" s="67"/>
       <c r="G3" s="67"/>
@@ -1998,22 +1637,22 @@
       <c r="Q4" s="10"/>
     </row>
     <row r="5" spans="3:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="96" t="s">
-        <v>16</v>
+      <c r="C5" s="76" t="s">
+        <v>2</v>
       </c>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="97"/>
-      <c r="H5" s="97"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="97"/>
-      <c r="K5" s="97"/>
-      <c r="L5" s="97"/>
-      <c r="M5" s="97"/>
-      <c r="N5" s="97"/>
-      <c r="O5" s="97"/>
-      <c r="P5" s="98"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="77"/>
+      <c r="N5" s="77"/>
+      <c r="O5" s="77"/>
+      <c r="P5" s="78"/>
       <c r="Q5" s="10"/>
     </row>
     <row r="6" spans="3:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2034,118 +1673,120 @@
       <c r="Q6" s="10"/>
     </row>
     <row r="7" spans="3:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C7" s="75" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="76"/>
-      <c r="E7" s="76"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="78" t="s">
+      <c r="C7" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="76"/>
-      <c r="I7" s="76"/>
-      <c r="J7" s="76"/>
-      <c r="K7" s="77"/>
-      <c r="L7" s="78" t="s">
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="M7" s="76"/>
-      <c r="N7" s="76"/>
-      <c r="O7" s="76"/>
-      <c r="P7" s="79"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
+      <c r="O7" s="74"/>
+      <c r="P7" s="80"/>
       <c r="Q7" s="10"/>
     </row>
     <row r="8" spans="3:17" ht="57" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="C8" s="99"/>
-      <c r="D8" s="100"/>
-      <c r="E8" s="100"/>
-      <c r="F8" s="101"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="83"/>
       <c r="G8" s="52" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="H8" s="44"/>
       <c r="I8" s="44" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="J8" s="44"/>
       <c r="K8" s="45" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
-      <c r="L8" s="102" t="s">
-        <v>22</v>
+      <c r="L8" s="84" t="s">
+        <v>9</v>
       </c>
-      <c r="M8" s="103"/>
-      <c r="N8" s="103"/>
-      <c r="O8" s="103"/>
-      <c r="P8" s="104"/>
+      <c r="M8" s="85"/>
+      <c r="N8" s="85"/>
+      <c r="O8" s="85"/>
+      <c r="P8" s="86"/>
       <c r="Q8" s="10"/>
     </row>
     <row r="9" spans="3:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C9" s="75" t="s">
-        <v>0</v>
+      <c r="C9" s="73" t="s">
+        <v>10</v>
       </c>
-      <c r="D9" s="76"/>
-      <c r="E9" s="76"/>
-      <c r="F9" s="77"/>
-      <c r="G9" s="78" t="s">
-        <v>23</v>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="79" t="s">
+        <v>11</v>
       </c>
-      <c r="H9" s="76"/>
-      <c r="I9" s="76"/>
-      <c r="J9" s="76"/>
-      <c r="K9" s="77"/>
-      <c r="L9" s="78" t="s">
-        <v>1</v>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="75"/>
+      <c r="L9" s="79" t="s">
+        <v>12</v>
       </c>
-      <c r="M9" s="77"/>
-      <c r="N9" s="78" t="s">
-        <v>26</v>
+      <c r="M9" s="75"/>
+      <c r="N9" s="79" t="s">
+        <v>13</v>
       </c>
-      <c r="O9" s="76"/>
-      <c r="P9" s="79"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="80"/>
       <c r="Q9" s="10"/>
     </row>
     <row r="10" spans="3:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="C10" s="99"/>
-      <c r="D10" s="100"/>
-      <c r="E10" s="100"/>
-      <c r="F10" s="101"/>
-      <c r="G10" s="80"/>
-      <c r="H10" s="81"/>
-      <c r="I10" s="81"/>
-      <c r="J10" s="81"/>
-      <c r="K10" s="82"/>
-      <c r="L10" s="86"/>
-      <c r="M10" s="87"/>
-      <c r="N10" s="83"/>
-      <c r="O10" s="84"/>
-      <c r="P10" s="85"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="87"/>
+      <c r="H10" s="88"/>
+      <c r="I10" s="88"/>
+      <c r="J10" s="88"/>
+      <c r="K10" s="89"/>
+      <c r="L10" s="93"/>
+      <c r="M10" s="94"/>
+      <c r="N10" s="90"/>
+      <c r="O10" s="91"/>
+      <c r="P10" s="92"/>
       <c r="Q10" s="10"/>
     </row>
     <row r="11" spans="3:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C11" s="13"/>
-      <c r="D11" s="76" t="s">
-        <v>27</v>
+      <c r="D11" s="74" t="s">
+        <v>14</v>
       </c>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="76"/>
-      <c r="H11" s="76"/>
-      <c r="I11" s="77"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="75"/>
       <c r="J11" s="11"/>
-      <c r="K11" s="78" t="s">
-        <v>27</v>
+      <c r="K11" s="79" t="s">
+        <v>14</v>
       </c>
-      <c r="L11" s="76"/>
-      <c r="M11" s="76"/>
-      <c r="N11" s="76"/>
-      <c r="O11" s="76"/>
-      <c r="P11" s="77"/>
+      <c r="L11" s="74"/>
+      <c r="M11" s="74"/>
+      <c r="N11" s="74"/>
+      <c r="O11" s="74"/>
+      <c r="P11" s="75"/>
       <c r="Q11" s="10"/>
     </row>
-    <row r="12" spans="3:17" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C12" s="68"/>
+    <row r="12" spans="3:17" ht="46.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C12" s="68" t="s">
+        <v>15</v>
+      </c>
       <c r="D12" s="69"/>
       <c r="E12" s="69"/>
       <c r="F12" s="69"/>
@@ -2153,7 +1794,9 @@
       <c r="H12" s="70"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
-      <c r="K12" s="68"/>
+      <c r="K12" s="68" t="s">
+        <v>16</v>
+      </c>
       <c r="L12" s="69"/>
       <c r="M12" s="69"/>
       <c r="N12" s="69"/>
@@ -2161,58 +1804,58 @@
       <c r="P12" s="70"/>
       <c r="Q12" s="10"/>
     </row>
-    <row r="13" spans="3:17" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="3:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C13" s="15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D13" s="71" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E13" s="72"/>
       <c r="F13" s="16" t="s">
         <v>19</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="J13" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" s="72"/>
+      <c r="M13" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="N13" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="K13" s="73" t="s">
-        <v>6</v>
-      </c>
-      <c r="L13" s="74"/>
-      <c r="M13" s="16" t="s">
+      <c r="O13" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="N13" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="O13" s="16" t="s">
-        <v>8</v>
-      </c>
       <c r="P13" s="16" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="Q13" s="10"/>
     </row>
-    <row r="14" spans="3:17" ht="28.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="3:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C14" s="21"/>
-      <c r="D14" s="94"/>
-      <c r="E14" s="95"/>
+      <c r="D14" s="101"/>
+      <c r="E14" s="102"/>
       <c r="F14" s="54"/>
       <c r="G14" s="12"/>
       <c r="H14" s="22"/>
       <c r="I14" s="12"/>
       <c r="J14" s="21"/>
-      <c r="K14" s="105"/>
-      <c r="L14" s="106"/>
+      <c r="K14" s="101"/>
+      <c r="L14" s="102"/>
       <c r="M14" s="54"/>
       <c r="N14" s="22"/>
       <c r="O14" s="22"/>
@@ -2491,7 +2134,7 @@
       <c r="P30" s="20"/>
       <c r="Q30" s="10"/>
       <c r="U30" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="3:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -2630,52 +2273,52 @@
       <c r="P38" s="23"/>
       <c r="Q38" s="10"/>
     </row>
-    <row r="39" spans="1:17" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C39" s="57"/>
-      <c r="D39" s="110"/>
-      <c r="E39" s="111"/>
+      <c r="D39" s="106"/>
+      <c r="E39" s="107"/>
       <c r="F39" s="58"/>
       <c r="G39" s="59"/>
       <c r="H39" s="59"/>
       <c r="I39" s="59"/>
       <c r="J39" s="57"/>
-      <c r="K39" s="110"/>
-      <c r="L39" s="111"/>
+      <c r="K39" s="106"/>
+      <c r="L39" s="107"/>
       <c r="M39" s="60"/>
       <c r="N39" s="59"/>
       <c r="O39" s="59"/>
       <c r="P39" s="61"/>
       <c r="Q39" s="10"/>
     </row>
-    <row r="40" spans="1:17" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C40" s="26"/>
       <c r="D40" s="62" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E40" s="63"/>
       <c r="F40" s="64" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G40" s="62"/>
       <c r="H40" s="62"/>
       <c r="I40" s="62"/>
       <c r="J40" s="62"/>
-      <c r="K40" s="107" t="s">
-        <v>9</v>
+      <c r="K40" s="103" t="s">
+        <v>26</v>
       </c>
-      <c r="L40" s="108"/>
-      <c r="M40" s="108" t="s">
-        <v>10</v>
+      <c r="L40" s="104"/>
+      <c r="M40" s="104" t="s">
+        <v>27</v>
       </c>
-      <c r="N40" s="108"/>
-      <c r="O40" s="108"/>
-      <c r="P40" s="109"/>
+      <c r="N40" s="104"/>
+      <c r="O40" s="104"/>
+      <c r="P40" s="105"/>
       <c r="Q40" s="32"/>
     </row>
-    <row r="41" spans="1:17" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C41" s="88"/>
-      <c r="D41" s="89"/>
-      <c r="E41" s="90"/>
+    <row r="41" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C41" s="95"/>
+      <c r="D41" s="96"/>
+      <c r="E41" s="97"/>
       <c r="F41" s="46"/>
       <c r="G41" s="47"/>
       <c r="H41" s="47"/>
@@ -2689,9 +2332,9 @@
       <c r="P41" s="49"/>
       <c r="Q41" s="30"/>
     </row>
-    <row r="42" spans="1:17" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C42" s="50" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D42" s="34"/>
       <c r="E42" s="35"/>
@@ -2701,7 +2344,7 @@
       <c r="I42" s="34"/>
       <c r="J42" s="34"/>
       <c r="K42" s="36" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="L42" s="35"/>
       <c r="M42" s="36"/>
@@ -2710,10 +2353,10 @@
       <c r="P42" s="37"/>
       <c r="Q42" s="30"/>
     </row>
-    <row r="43" spans="1:17" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:17" ht="44.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C43" s="38"/>
       <c r="D43" s="28" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
@@ -2722,13 +2365,13 @@
       <c r="I43" s="28"/>
       <c r="J43" s="28"/>
       <c r="K43" s="27" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="L43" s="28"/>
-      <c r="M43" s="91"/>
-      <c r="N43" s="92"/>
-      <c r="O43" s="92"/>
-      <c r="P43" s="93"/>
+      <c r="M43" s="98"/>
+      <c r="N43" s="99"/>
+      <c r="O43" s="99"/>
+      <c r="P43" s="100"/>
       <c r="Q43" s="30"/>
     </row>
     <row r="44" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -2804,19 +2447,19 @@
       <c r="B48" s="1"/>
       <c r="C48" s="31"/>
       <c r="D48" s="32" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="E48" s="32"/>
       <c r="F48" s="32"/>
       <c r="G48" s="32" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="H48" s="32"/>
       <c r="I48" s="32"/>
       <c r="J48" s="32"/>
       <c r="K48" s="32"/>
       <c r="L48" s="32" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="M48" s="32"/>
       <c r="N48" s="32"/>
@@ -2858,7 +2501,7 @@
       <c r="P50" s="40"/>
       <c r="Q50" s="30"/>
     </row>
-    <row r="51" spans="3:17" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="3:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C51" s="41"/>
       <c r="D51" s="42"/>
       <c r="E51" s="42"/>
@@ -2875,7 +2518,7 @@
       <c r="P51" s="43"/>
       <c r="Q51" s="30"/>
     </row>
-    <row r="52" spans="3:17" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C52" s="39"/>
       <c r="D52" s="39"/>
       <c r="E52" s="39"/>
@@ -6582,6 +6225,7 @@
       <c r="Q269" s="10"/>
     </row>
   </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="77">
     <mergeCell ref="K39:L39"/>
     <mergeCell ref="C10:F10"/>
@@ -6590,6 +6234,15 @@
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="K16:L16"/>
     <mergeCell ref="D23:E23"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D28:E28"/>
     <mergeCell ref="M43:P43"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D19:E19"/>
@@ -6611,15 +6264,14 @@
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="D37:E37"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="N9:P9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="G10:K10"/>
     <mergeCell ref="N10:P10"/>
     <mergeCell ref="L10:M10"/>
     <mergeCell ref="G9:K9"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="K28:L28"/>
     <mergeCell ref="E3:L3"/>
     <mergeCell ref="C12:H12"/>
     <mergeCell ref="K12:P12"/>
@@ -6632,19 +6284,7 @@
     <mergeCell ref="L7:P7"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="L8:P8"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="N9:P9"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D21:E21"/>
@@ -6660,13 +6300,14 @@
     <mergeCell ref="K22:L22"/>
     <mergeCell ref="K21:L21"/>
     <mergeCell ref="K32:L32"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="K30:L30"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0" right="0" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0.11811023622047245"/>
-  <pageSetup paperSize="5" scale="65" orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="M40:P40 N39:P39" numberStoredAsText="1"/>
-  </ignoredErrors>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0" right="0" top="0.19685039370078999" bottom="0.19685039370078999" header="0" footer="0.11811023622047"/>
+  <pageSetup paperSize="5" scale="65" orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>